<commit_message>
Update hypertension to remove diabetes reference
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_hypertension_dyn.xlsx
+++ b/tests/databooks/databook_hypertension_dyn.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/databooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh.abey\Desktop\projects\atomica\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A06483B7-72A7-E542-943A-31C38DEFF014}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10700" yWindow="460" windowWidth="19140" windowHeight="14420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10698" yWindow="462" windowWidth="19140" windowHeight="14418" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -21,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{9B9FFBF5-96F1-FB4E-891C-4F7C6DD697CA}">
+    <comment ref="E8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{AA84D980-2417-EA49-B771-8075726DEED2}">
+    <comment ref="E9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -112,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{F15B674C-D29E-0D45-9327-45E7C2D94A27}">
+    <comment ref="E10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{2E8C33C0-7ED9-E44D-9C68-D75D509BCC6A}">
+    <comment ref="E11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -198,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{2F35E008-FCB7-8243-9461-D063C8B2212C}">
+    <comment ref="E14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -241,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{E5FE5A21-3B5D-4D4F-BDC8-B6E3B11E15C6}">
+    <comment ref="E15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -284,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E16" authorId="0" shapeId="0" xr:uid="{9E1B0647-5CDB-AB49-95B9-202841356ADD}">
+    <comment ref="E16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -327,7 +326,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E17" authorId="0" shapeId="0" xr:uid="{EECAB18B-A0A8-D843-94A1-EE4BAB9C4A96}">
+    <comment ref="E17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -370,7 +369,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{EB3E8A7A-A60C-E24F-A6DA-A3E9345B973E}">
+    <comment ref="E20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -413,7 +412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E21" authorId="0" shapeId="0" xr:uid="{E34D991F-1B09-7740-B9E3-8948A9E945DF}">
+    <comment ref="E21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -456,7 +455,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{CC9CF311-F570-A74F-85EC-7E45BA56F45C}">
+    <comment ref="E22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -499,7 +498,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E23" authorId="0" shapeId="0" xr:uid="{EF8A4844-8BF6-DB4B-8181-DE5D96D9DE58}">
+    <comment ref="E23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -542,7 +541,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E26" authorId="0" shapeId="0" xr:uid="{164BBDB8-5A08-6548-BEFA-50B4C7B9CDD8}">
+    <comment ref="E26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -585,7 +584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E27" authorId="0" shapeId="0" xr:uid="{04F55A7F-D604-104D-B994-2D29490B1090}">
+    <comment ref="E27" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -628,7 +627,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E28" authorId="0" shapeId="0" xr:uid="{534125C3-8659-074D-AC8E-D3DD363A896B}">
+    <comment ref="E28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -671,7 +670,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E29" authorId="0" shapeId="0" xr:uid="{C3A0EF00-32BA-3641-87EC-57403D89C488}">
+    <comment ref="E29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -714,7 +713,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E32" authorId="0" shapeId="0" xr:uid="{F2DCBA44-A5E6-5B46-9D97-66013B2B83F0}">
+    <comment ref="E32" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -757,7 +756,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E33" authorId="0" shapeId="0" xr:uid="{F89E787E-7220-5741-83E0-BC6A9D580559}">
+    <comment ref="E33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -800,7 +799,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E34" authorId="0" shapeId="0" xr:uid="{7A236FDC-2BE8-034E-A059-EFD93E78458A}">
+    <comment ref="E34" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -843,7 +842,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E35" authorId="0" shapeId="0" xr:uid="{F95812C9-AB7C-9A4D-BA18-10C70CDAEBCE}">
+    <comment ref="E35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -886,7 +885,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E44" authorId="0" shapeId="0" xr:uid="{722B68A5-7350-0442-8A9A-434636936955}">
+    <comment ref="E44" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -919,7 +918,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E45" authorId="0" shapeId="0" xr:uid="{786C846A-7FDA-1E49-B6C7-25D00B7BD7A1}">
+    <comment ref="E45" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -952,7 +951,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E46" authorId="0" shapeId="0" xr:uid="{27AAF8D6-CA27-BA4D-A850-6FC1E3223764}">
+    <comment ref="E46" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -985,7 +984,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E47" authorId="0" shapeId="0" xr:uid="{0D65036E-A9BD-E149-B942-1998E72B2C76}">
+    <comment ref="E47" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1018,7 +1017,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E50" authorId="0" shapeId="0" xr:uid="{3FF4C394-700E-CF45-9E00-1F45FCA3FF11}">
+    <comment ref="E50" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1051,7 +1050,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E51" authorId="0" shapeId="0" xr:uid="{A2536B07-8F21-FD46-81D7-0A6F97272204}">
+    <comment ref="E51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1084,7 +1083,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E52" authorId="0" shapeId="0" xr:uid="{8A69AA3D-D588-D848-87FE-B538E8E1855C}">
+    <comment ref="E52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1117,7 +1116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E53" authorId="0" shapeId="0" xr:uid="{1F9D980B-429F-F542-8C92-66D72B2F2472}">
+    <comment ref="E53" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1150,7 +1149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E56" authorId="0" shapeId="0" xr:uid="{F6653CB7-D167-4E43-A9E7-B413FA42A4D8}">
+    <comment ref="E56" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1183,7 +1182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E57" authorId="0" shapeId="0" xr:uid="{18F619CE-F770-F946-A05C-32A12976EF53}">
+    <comment ref="E57" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1216,7 +1215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E58" authorId="0" shapeId="0" xr:uid="{90B4A574-D976-1D41-9E3C-398A60EBECA2}">
+    <comment ref="E58" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1249,7 +1248,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E59" authorId="0" shapeId="0" xr:uid="{1A3D7A89-0CF1-134F-83AC-EB24D680EC6C}">
+    <comment ref="E59" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1282,7 +1281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E62" authorId="0" shapeId="0" xr:uid="{A37F57AD-7B4A-8B40-80AA-9724F2478A74}">
+    <comment ref="E62" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1315,7 +1314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E63" authorId="0" shapeId="0" xr:uid="{77985801-AA79-0143-AEDF-E62E5C7D5403}">
+    <comment ref="E63" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1348,7 +1347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E64" authorId="0" shapeId="0" xr:uid="{721E83C6-48A2-1C40-B6C3-1F5E243C58A0}">
+    <comment ref="E64" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1381,7 +1380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E65" authorId="0" shapeId="0" xr:uid="{19094C0B-112F-AE4E-B627-872E1B61B5DA}">
+    <comment ref="E65" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1414,7 +1413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E68" authorId="0" shapeId="0" xr:uid="{1A6CFAE8-A9C3-E44F-854F-8DD21757C28B}">
+    <comment ref="E68" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1447,7 +1446,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E69" authorId="0" shapeId="0" xr:uid="{81518AB7-5D30-214E-990C-162CF72FAF98}">
+    <comment ref="E69" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1480,7 +1479,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E70" authorId="0" shapeId="0" xr:uid="{314D0511-7717-D246-9042-75B678D3C0E6}">
+    <comment ref="E70" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1513,7 +1512,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E71" authorId="0" shapeId="0" xr:uid="{58657CE6-FF0E-324F-860A-7AED04FF47AB}">
+    <comment ref="E71" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1590,9 +1589,6 @@
   </si>
   <si>
     <t>Annual number of births</t>
-  </si>
-  <si>
-    <t>Estimated number of new diabetes cases annually</t>
   </si>
   <si>
     <t>Annual number screened</t>
@@ -1648,11 +1644,14 @@
   <si>
     <t>Urban females</t>
   </si>
+  <si>
+    <t>Estimated number of new cases annually</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2635,23 +2634,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2687,23 +2669,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2879,7 +2844,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -2889,12 +2854,12 @@
       <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="14.83203125" customWidth="1"/>
+    <col min="1" max="2" width="14.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2902,36 +2867,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2940,25 +2905,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="68.83203125" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="3.83203125" customWidth="1"/>
+    <col min="1" max="1" width="68.83984375" customWidth="1"/>
+    <col min="2" max="2" width="13.83984375" customWidth="1"/>
+    <col min="3" max="3" width="10.47265625" customWidth="1"/>
+    <col min="4" max="4" width="3.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2982,7 +2947,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>m_rural</v>
@@ -3002,7 +2967,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>f_rural</v>
@@ -3022,7 +2987,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>m_urban</v>
@@ -3043,7 +3008,7 @@
       <c r="H4" s="2"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>f_urban</v>
@@ -3063,7 +3028,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -3087,7 +3052,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>m_rural</v>
@@ -3106,7 +3071,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>f_rural</v>
@@ -3125,7 +3090,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>m_urban</v>
@@ -3144,7 +3109,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>f_urban</v>
@@ -3163,7 +3128,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -3187,7 +3152,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>m_rural</v>
@@ -3206,7 +3171,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>f_rural</v>
@@ -3225,7 +3190,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>m_urban</v>
@@ -3244,7 +3209,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>f_urban</v>
@@ -3263,7 +3228,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -3287,7 +3252,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>m_rural</v>
@@ -3306,7 +3271,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>f_rural</v>
@@ -3325,7 +3290,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>m_urban</v>
@@ -3344,7 +3309,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>f_urban</v>
@@ -3363,7 +3328,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -3387,7 +3352,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>m_rural</v>
@@ -3406,7 +3371,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>f_rural</v>
@@ -3425,7 +3390,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>m_urban</v>
@@ -3444,7 +3409,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>f_urban</v>
@@ -3463,7 +3428,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -3487,7 +3452,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>m_rural</v>
@@ -3506,7 +3471,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>f_rural</v>
@@ -3525,7 +3490,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>m_urban</v>
@@ -3544,7 +3509,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>f_urban</v>
@@ -3563,7 +3528,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
@@ -3587,7 +3552,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>m_rural</v>
@@ -3607,7 +3572,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>f_rural</v>
@@ -3627,7 +3592,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>m_urban</v>
@@ -3647,7 +3612,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>f_urban</v>
@@ -3667,9 +3632,9 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>3</v>
@@ -3691,7 +3656,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>m_rural</v>
@@ -3710,7 +3675,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>f_rural</v>
@@ -3729,7 +3694,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>m_urban</v>
@@ -3748,7 +3713,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>f_urban</v>
@@ -3767,9 +3732,9 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>3</v>
@@ -3791,7 +3756,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>m_rural</v>
@@ -3811,7 +3776,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>f_rural</v>
@@ -3831,7 +3796,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>m_urban</v>
@@ -3851,7 +3816,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>f_urban</v>
@@ -3871,9 +3836,9 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>3</v>
@@ -3895,7 +3860,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>m_rural</v>
@@ -3914,7 +3879,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>f_rural</v>
@@ -3933,7 +3898,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>m_urban</v>
@@ -3952,7 +3917,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>f_urban</v>
@@ -3971,9 +3936,9 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>3</v>
@@ -3995,7 +3960,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>m_rural</v>
@@ -4014,7 +3979,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>f_rural</v>
@@ -4033,7 +3998,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>m_urban</v>
@@ -4052,7 +4017,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>f_urban</v>
@@ -4071,9 +4036,9 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>3</v>
@@ -4095,13 +4060,13 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>m_rural</v>
       </c>
       <c r="B68" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="3" t="s">
@@ -4114,13 +4079,13 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>f_rural</v>
       </c>
       <c r="B69" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="3" t="s">
@@ -4133,13 +4098,13 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>m_urban</v>
       </c>
       <c r="B70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="3" t="s">
@@ -4152,13 +4117,13 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>f_urban</v>
       </c>
       <c r="B71" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="3" t="s">
@@ -4171,9 +4136,9 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>3</v>
@@ -4195,13 +4160,13 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>m_rural</v>
       </c>
       <c r="B74" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C74" s="4">
         <v>0.2</v>
@@ -4214,13 +4179,13 @@
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>f_rural</v>
       </c>
       <c r="B75" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C75" s="4">
         <v>0.2</v>
@@ -4233,13 +4198,13 @@
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>m_urban</v>
       </c>
       <c r="B76" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C76" s="4">
         <v>0.2</v>
@@ -4252,13 +4217,13 @@
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>f_urban</v>
       </c>
       <c r="B77" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C77" s="4">
         <v>0.2</v>
@@ -4271,9 +4236,9 @@
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>3</v>
@@ -4295,13 +4260,13 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>m_rural</v>
       </c>
       <c r="B80" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C80" s="4">
         <v>0.16</v>
@@ -4314,13 +4279,13 @@
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>f_rural</v>
       </c>
       <c r="B81" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C81" s="4">
         <v>0.16</v>
@@ -4333,13 +4298,13 @@
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>m_urban</v>
       </c>
       <c r="B82" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C82" s="4">
         <v>0.16</v>
@@ -4352,13 +4317,13 @@
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>f_urban</v>
       </c>
       <c r="B83" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C83" s="4">
         <v>0.16</v>
@@ -4371,9 +4336,9 @@
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>3</v>
@@ -4395,13 +4360,13 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>m_rural</v>
       </c>
       <c r="B86" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C86" s="4">
         <v>2.5000000000000001E-2</v>
@@ -4414,13 +4379,13 @@
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>f_rural</v>
       </c>
       <c r="B87" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C87" s="4">
         <v>2.5000000000000001E-2</v>
@@ -4433,13 +4398,13 @@
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>m_urban</v>
       </c>
       <c r="B88" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C88" s="4">
         <v>2.5000000000000001E-2</v>
@@ -4452,13 +4417,13 @@
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>f_urban</v>
       </c>
       <c r="B89" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C89" s="4">
         <v>2.5000000000000001E-2</v>
@@ -4471,9 +4436,9 @@
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>3</v>
@@ -4495,13 +4460,13 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>m_rural</v>
       </c>
       <c r="B92" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C92" s="4">
         <v>1.4999999999999999E-2</v>
@@ -4514,13 +4479,13 @@
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>f_rural</v>
       </c>
       <c r="B93" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C93" s="4">
         <v>1.4999999999999999E-2</v>
@@ -4533,13 +4498,13 @@
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>m_urban</v>
       </c>
       <c r="B94" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C94" s="4">
         <v>1.4999999999999999E-2</v>
@@ -4552,13 +4517,13 @@
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>f_urban</v>
       </c>
       <c r="B95" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C95" s="4">
         <v>1.4999999999999999E-2</v>
@@ -5085,13 +5050,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B62:B65 B56:B59 B50:B53 B44:B47 B38:B41 B32:B35 B26:B29 B20:B23 B14:B17 B8:B11 B2:B5" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B62:B65 B56:B59 B50:B53 B44:B47 B38:B41 B32:B35 B26:B29 B20:B23 B14:B17 B8:B11 B2:B5">
       <formula1>"Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B92:B95 B86:B89 B80:B83 B68:B71" xr:uid="{00000000-0002-0000-0100-00002C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B92:B95 B86:B89 B80:B83 B68:B71">
       <formula1>"Probability"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74:B77" xr:uid="{00000000-0002-0000-0100-000030000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74:B77">
       <formula1>"Duration"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>